<commit_message>
Updated read me file
</commit_message>
<xml_diff>
--- a/src/main/resources/howtodoinjava_demo.xlsx
+++ b/src/main/resources/howtodoinjava_demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lokes\IdeaProjects\opensource-examples\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C223E539-11B7-4D81-BDF5-932A3742DEDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86013D11-B46F-4952-9A33-D42C44095C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4308" yWindow="2100" windowWidth="17280" windowHeight="6540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee Data" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -104,8 +110,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,63 +435,66 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -493,40 +508,43 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="9.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>